<commit_message>
Penambahan input kecamatan, kelurahan, kota dan kode pos di module Customer
</commit_message>
<xml_diff>
--- a/format file import/File Import Excel/Master Data/data_customer.xlsx
+++ b/format file import/File Import Excel/Master Data/data_customer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>KETERANGAN INPUT DATA MELALUI EXCEL</t>
   </si>
@@ -54,6 +54,18 @@
   </si>
   <si>
     <t>Jika melanggar ketentuan di atas, proses import data akan gagal</t>
+  </si>
+  <si>
+    <t>KELURAHAN</t>
+  </si>
+  <si>
+    <t>KECAMATAN</t>
+  </si>
+  <si>
+    <t>KOTA</t>
+  </si>
+  <si>
+    <t>KODE POS</t>
   </si>
 </sst>
 </file>
@@ -469,22 +481,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="16.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -492,12 +506,24 @@
         <v>10</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve form customer: * Penambahan pilihan jenis customer (semua, umum dan reseller) * Penambahan fitur pencarian nama customer
</commit_message>
<xml_diff>
--- a/format file import/File Import Excel/Master Data/data_customer.xlsx
+++ b/format file import/File Import Excel/Master Data/data_customer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>KETERANGAN INPUT DATA MELALUI EXCEL</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>KODE POS</t>
+  </si>
+  <si>
+    <t>DISKON RESELLER</t>
   </si>
 </sst>
 </file>
@@ -481,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,10 +498,11 @@
     <col min="6" max="6" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -524,6 +528,9 @@
         <v>9</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Penambahan input kecamatan dan kabupaten di module customer
</commit_message>
<xml_diff>
--- a/format file import/File Import Excel/Master Data/data_customer.xlsx
+++ b/format file import/File Import Excel/Master Data/data_customer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>KETERANGAN INPUT DATA MELALUI EXCEL</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>DISKON RESELLER</t>
+  </si>
+  <si>
+    <t>DESA</t>
+  </si>
+  <si>
+    <t>KABUPATEN</t>
   </si>
 </sst>
 </file>
@@ -484,25 +490,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="16.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="16.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -510,27 +516,33 @@
         <v>10</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed issues: * Penambahan data master wilayah (provinsi, kabupaten dan kecamatan) * Penyesuaian module customer untuk data wilayah
</commit_message>
<xml_diff>
--- a/format file import/File Import Excel/Master Data/data_customer.xlsx
+++ b/format file import/File Import Excel/Master Data/data_customer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>KETERANGAN INPUT DATA MELALUI EXCEL</t>
   </si>
@@ -56,32 +56,79 @@
     <t>Jika melanggar ketentuan di atas, proses import data akan gagal</t>
   </si>
   <si>
-    <t>KELURAHAN</t>
-  </si>
-  <si>
     <t>KECAMATAN</t>
   </si>
   <si>
-    <t>KOTA</t>
-  </si>
-  <si>
     <t>KODE POS</t>
   </si>
   <si>
     <t>DISKON RESELLER</t>
   </si>
   <si>
-    <t>DESA</t>
-  </si>
-  <si>
-    <t>KABUPATEN</t>
+    <t>PROVINSI</t>
+  </si>
+  <si>
+    <t>KABUPATEN/KOTA</t>
+  </si>
+  <si>
+    <t>KOLOM</t>
+  </si>
+  <si>
+    <t>Contoh: Kab. Sleman atau Kota Yogyakarta</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Untuk penulisan kabupaten/kota, tambahkan kata </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kab.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kota</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> di depan Nama kabupaten/kota</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +147,22 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -164,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -186,6 +249,10 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -490,59 +557,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="16.28515625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="21.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -554,23 +614,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="85.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -601,7 +661,29 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -610,5 +692,6 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>